<commit_message>
some of the links and scripts in Contact Me page is not working like bootstrap, javascript and font awesome that makes the site not functional
The links and script in Contact Me page has .min version in src and href that in files we don’t have the minimized version of the code
</commit_message>
<xml_diff>
--- a/Template-SEO-audit.xlsx
+++ b/Template-SEO-audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hamed Javedan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B011B38B-FF52-4A4C-B201-3EFFF6123D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7113FB19-A457-47D9-A230-511CD4A2A0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
   <si>
     <t>Category</t>
   </si>
@@ -183,9 +183,6 @@
     <t>The page does not contain a heading, skip link, or landmark region</t>
   </si>
   <si>
-    <t>adding a h4 tag on Toggle navigation</t>
-  </si>
-  <si>
     <t>https://web.dev/bypass/?utm_source=lighthouse&amp;utm_medium=devtools</t>
   </si>
   <si>
@@ -232,6 +229,21 @@
   </si>
   <si>
     <t>https://developer.mozilla.org/en-US/docs/Glossary/minification</t>
+  </si>
+  <si>
+    <t>adding a h2 tag on Let's talk web design!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some of the links and scripts in Contact Me page is not working like bootstrap, javascript and font awesome that makes the site not functional </t>
+  </si>
+  <si>
+    <t>The links and script in Contact Me page has .min version in src and href that in files we don’t have the minimized version of the code</t>
+  </si>
+  <si>
+    <t>I recommend to delete all .min from all the links that has this word in order to make the codes apply to the page  since we have the codes that are not minimized</t>
+  </si>
+  <si>
+    <t>We don't need a Reference for this problem since its just a typing mistake and there is no minimized version of the code</t>
   </si>
 </sst>
 </file>
@@ -585,18 +597,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="35.21875" customWidth="1"/>
-    <col min="3" max="3" width="70.44140625" customWidth="1"/>
+    <col min="2" max="2" width="109.5546875" customWidth="1"/>
+    <col min="3" max="3" width="104.109375" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" customWidth="1"/>
-    <col min="6" max="6" width="82.33203125" customWidth="1"/>
+    <col min="5" max="5" width="116.77734375" customWidth="1"/>
+    <col min="6" max="6" width="92.88671875" customWidth="1"/>
     <col min="7" max="26" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -753,10 +765,10 @@
         <v>33</v>
       </c>
       <c r="E8" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" t="s">
         <v>34</v>
-      </c>
-      <c r="F8" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1">
@@ -764,16 +776,16 @@
         <v>10</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="F9" t="s">
         <v>37</v>
-      </c>
-      <c r="F9" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1">
@@ -781,16 +793,16 @@
         <v>11</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="F10" t="s">
         <v>40</v>
-      </c>
-      <c r="F10" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
@@ -798,16 +810,16 @@
         <v>11</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>46</v>
-      </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
@@ -815,20 +827,34 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="E12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" t="s">
         <v>49</v>
       </c>
-      <c r="F12" t="s">
-        <v>50</v>
-      </c>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="E13" s="4"/>
+    <row r="13" spans="1:26" ht="16.5" customHeight="1">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
       <c r="E14" s="4"/>

</xml_diff>